<commit_message>
Added login test case
</commit_message>
<xml_diff>
--- a/TestData/Datafile.xlsx
+++ b/TestData/Datafile.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="1935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="logindata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A3:I6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,19 +21,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sunglass</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>otp</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>test91@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,13 +82,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -341,7 +377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -353,4 +389,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9582957891</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="test@123"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>